<commit_message>
Added first successful test case
</commit_message>
<xml_diff>
--- a/build/resources/test/data/DataSheet.xlsx
+++ b/build/resources/test/data/DataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09FB026-1CF1-4E23-91F7-AC505BF6406B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36823BEF-7206-44D2-A289-6F3914AE3BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1570" windowWidth="20470" windowHeight="8630" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="0" yWindow="1420" windowWidth="19200" windowHeight="8630" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="ImpactData" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>TCID</t>
   </si>
@@ -58,9 +58,6 @@
     <t>ExpectedResponseBody</t>
   </si>
   <si>
-    <t>/impacts/v1/impacts?startDate=2020-5-1&amp;endDate=2022-5-1</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
@@ -74,6 +71,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>impacts/v1/impacts?startDate=2020-5-1&amp;endDate=2022-5-1</t>
+  </si>
+  <si>
+    <t>400</t>
   </si>
 </sst>
 </file>
@@ -430,7 +433,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -450,7 +453,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -476,16 +479,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -493,16 +499,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>